<commit_message>
Reversed kth element - Not optimized
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1665,11 +1665,11 @@
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C66" activeCellId="0" sqref="C66"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B127" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C140" activeCellId="0" sqref="C140"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.55859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="123"/>
@@ -3123,7 +3123,7 @@
         <v>138</v>
       </c>
       <c r="C140" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
two stack in one array
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1665,11 +1665,11 @@
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B127" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C140" activeCellId="0" sqref="C140"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B286" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B299" activeCellId="0" sqref="B299"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.55859375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="123"/>
@@ -4789,7 +4789,7 @@
         <v>290</v>
       </c>
       <c r="C298" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
binary tree order level traversal
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="467">
   <si>
     <t xml:space="preserve">Questions by Love Babbar:</t>
   </si>
@@ -545,6 +545,9 @@
   </si>
   <si>
     <t xml:space="preserve">level order traversal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
   </si>
   <si>
     <t xml:space="preserve">Reverse Level Order traversal</t>
@@ -1665,11 +1668,11 @@
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B286" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B299" activeCellId="0" sqref="B299"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A169" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D177" activeCellId="0" sqref="D177"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="123"/>
@@ -3512,7 +3515,7 @@
         <v>174</v>
       </c>
       <c r="C177" s="5" t="s">
-        <v>5</v>
+        <v>175</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3520,7 +3523,7 @@
         <v>173</v>
       </c>
       <c r="B178" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C178" s="5" t="s">
         <v>5</v>
@@ -3531,7 +3534,7 @@
         <v>173</v>
       </c>
       <c r="B179" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C179" s="5" t="s">
         <v>5</v>
@@ -3542,7 +3545,7 @@
         <v>173</v>
       </c>
       <c r="B180" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C180" s="5" t="s">
         <v>5</v>
@@ -3553,7 +3556,7 @@
         <v>173</v>
       </c>
       <c r="B181" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C181" s="5" t="s">
         <v>5</v>
@@ -3564,7 +3567,7 @@
         <v>173</v>
       </c>
       <c r="B182" s="7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C182" s="5" t="s">
         <v>5</v>
@@ -3575,7 +3578,7 @@
         <v>173</v>
       </c>
       <c r="B183" s="7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C183" s="5" t="s">
         <v>5</v>
@@ -3586,7 +3589,7 @@
         <v>173</v>
       </c>
       <c r="B184" s="7" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C184" s="5" t="s">
         <v>5</v>
@@ -3597,7 +3600,7 @@
         <v>173</v>
       </c>
       <c r="B185" s="7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C185" s="5" t="s">
         <v>5</v>
@@ -3608,7 +3611,7 @@
         <v>173</v>
       </c>
       <c r="B186" s="7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C186" s="5" t="s">
         <v>5</v>
@@ -3619,7 +3622,7 @@
         <v>173</v>
       </c>
       <c r="B187" s="7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C187" s="5" t="s">
         <v>5</v>
@@ -3630,7 +3633,7 @@
         <v>173</v>
       </c>
       <c r="B188" s="7" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C188" s="5" t="s">
         <v>5</v>
@@ -3641,7 +3644,7 @@
         <v>173</v>
       </c>
       <c r="B189" s="7" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C189" s="5" t="s">
         <v>5</v>
@@ -3652,7 +3655,7 @@
         <v>173</v>
       </c>
       <c r="B190" s="7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C190" s="5" t="s">
         <v>5</v>
@@ -3663,7 +3666,7 @@
         <v>173</v>
       </c>
       <c r="B191" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C191" s="5" t="s">
         <v>5</v>
@@ -3674,7 +3677,7 @@
         <v>173</v>
       </c>
       <c r="B192" s="7" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C192" s="5" t="s">
         <v>5</v>
@@ -3685,7 +3688,7 @@
         <v>173</v>
       </c>
       <c r="B193" s="7" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C193" s="5" t="s">
         <v>5</v>
@@ -3696,7 +3699,7 @@
         <v>173</v>
       </c>
       <c r="B194" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C194" s="5" t="s">
         <v>5</v>
@@ -3707,7 +3710,7 @@
         <v>173</v>
       </c>
       <c r="B195" s="7" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C195" s="5" t="s">
         <v>5</v>
@@ -3718,7 +3721,7 @@
         <v>173</v>
       </c>
       <c r="B196" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C196" s="5" t="s">
         <v>5</v>
@@ -3729,7 +3732,7 @@
         <v>173</v>
       </c>
       <c r="B197" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C197" s="5" t="s">
         <v>5</v>
@@ -3740,7 +3743,7 @@
         <v>173</v>
       </c>
       <c r="B198" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C198" s="5" t="s">
         <v>5</v>
@@ -3751,7 +3754,7 @@
         <v>173</v>
       </c>
       <c r="B199" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C199" s="5" t="s">
         <v>5</v>
@@ -3762,7 +3765,7 @@
         <v>173</v>
       </c>
       <c r="B200" s="7" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C200" s="5" t="s">
         <v>5</v>
@@ -3773,7 +3776,7 @@
         <v>173</v>
       </c>
       <c r="B201" s="7" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C201" s="5" t="s">
         <v>5</v>
@@ -3784,7 +3787,7 @@
         <v>173</v>
       </c>
       <c r="B202" s="7" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C202" s="5" t="s">
         <v>5</v>
@@ -3795,7 +3798,7 @@
         <v>173</v>
       </c>
       <c r="B203" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C203" s="5" t="s">
         <v>5</v>
@@ -3806,7 +3809,7 @@
         <v>173</v>
       </c>
       <c r="B204" s="7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C204" s="5" t="s">
         <v>5</v>
@@ -3817,7 +3820,7 @@
         <v>173</v>
       </c>
       <c r="B205" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C205" s="5" t="s">
         <v>5</v>
@@ -3828,7 +3831,7 @@
         <v>173</v>
       </c>
       <c r="B206" s="7" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C206" s="5" t="s">
         <v>5</v>
@@ -3839,7 +3842,7 @@
         <v>173</v>
       </c>
       <c r="B207" s="7" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C207" s="5" t="s">
         <v>5</v>
@@ -3850,7 +3853,7 @@
         <v>173</v>
       </c>
       <c r="B208" s="7" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C208" s="5" t="s">
         <v>5</v>
@@ -3861,7 +3864,7 @@
         <v>173</v>
       </c>
       <c r="B209" s="7" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C209" s="5" t="s">
         <v>5</v>
@@ -3872,7 +3875,7 @@
         <v>173</v>
       </c>
       <c r="B210" s="7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C210" s="5" t="s">
         <v>5</v>
@@ -3883,7 +3886,7 @@
         <v>173</v>
       </c>
       <c r="B211" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C211" s="5" t="s">
         <v>5</v>
@@ -3901,10 +3904,10 @@
     </row>
     <row r="214" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B214" s="7" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C214" s="5" t="s">
         <v>5</v>
@@ -3912,10 +3915,10 @@
     </row>
     <row r="215" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B215" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C215" s="5" t="s">
         <v>5</v>
@@ -3923,10 +3926,10 @@
     </row>
     <row r="216" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B216" s="7" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C216" s="5" t="s">
         <v>5</v>
@@ -3934,10 +3937,10 @@
     </row>
     <row r="217" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B217" s="7" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C217" s="5" t="s">
         <v>5</v>
@@ -3945,10 +3948,10 @@
     </row>
     <row r="218" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B218" s="7" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C218" s="5" t="s">
         <v>5</v>
@@ -3956,10 +3959,10 @@
     </row>
     <row r="219" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B219" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C219" s="5" t="s">
         <v>5</v>
@@ -3967,10 +3970,10 @@
     </row>
     <row r="220" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B220" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C220" s="5" t="s">
         <v>5</v>
@@ -3978,10 +3981,10 @@
     </row>
     <row r="221" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B221" s="7" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C221" s="5" t="s">
         <v>5</v>
@@ -3989,10 +3992,10 @@
     </row>
     <row r="222" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B222" s="7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C222" s="5" t="s">
         <v>5</v>
@@ -4000,10 +4003,10 @@
     </row>
     <row r="223" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B223" s="7" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C223" s="5" t="s">
         <v>5</v>
@@ -4011,10 +4014,10 @@
     </row>
     <row r="224" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B224" s="7" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C224" s="5" t="s">
         <v>5</v>
@@ -4022,10 +4025,10 @@
     </row>
     <row r="225" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B225" s="7" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C225" s="5" t="s">
         <v>5</v>
@@ -4033,10 +4036,10 @@
     </row>
     <row r="226" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B226" s="7" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C226" s="5" t="s">
         <v>5</v>
@@ -4044,10 +4047,10 @@
     </row>
     <row r="227" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B227" s="7" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C227" s="5" t="s">
         <v>5</v>
@@ -4055,10 +4058,10 @@
     </row>
     <row r="228" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B228" s="7" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C228" s="5" t="s">
         <v>5</v>
@@ -4066,10 +4069,10 @@
     </row>
     <row r="229" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B229" s="7" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C229" s="5" t="s">
         <v>5</v>
@@ -4077,10 +4080,10 @@
     </row>
     <row r="230" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B230" s="7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C230" s="5" t="s">
         <v>5</v>
@@ -4088,10 +4091,10 @@
     </row>
     <row r="231" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B231" s="7" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C231" s="5" t="s">
         <v>5</v>
@@ -4099,10 +4102,10 @@
     </row>
     <row r="232" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B232" s="7" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C232" s="5" t="s">
         <v>5</v>
@@ -4110,10 +4113,10 @@
     </row>
     <row r="233" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B233" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C233" s="5" t="s">
         <v>5</v>
@@ -4121,10 +4124,10 @@
     </row>
     <row r="234" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B234" s="7" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C234" s="5" t="s">
         <v>5</v>
@@ -4132,10 +4135,10 @@
     </row>
     <row r="235" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B235" s="7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C235" s="5" t="s">
         <v>5</v>
@@ -4151,10 +4154,10 @@
     </row>
     <row r="238" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B238" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C238" s="5" t="s">
         <v>5</v>
@@ -4162,10 +4165,10 @@
     </row>
     <row r="239" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B239" s="7" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C239" s="5" t="s">
         <v>5</v>
@@ -4173,10 +4176,10 @@
     </row>
     <row r="240" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B240" s="7" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C240" s="5" t="s">
         <v>5</v>
@@ -4184,10 +4187,10 @@
     </row>
     <row r="241" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B241" s="7" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C241" s="5" t="s">
         <v>5</v>
@@ -4195,10 +4198,10 @@
     </row>
     <row r="242" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B242" s="7" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C242" s="5" t="s">
         <v>5</v>
@@ -4206,10 +4209,10 @@
     </row>
     <row r="243" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B243" s="7" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C243" s="5" t="s">
         <v>5</v>
@@ -4217,10 +4220,10 @@
     </row>
     <row r="244" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B244" s="7" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C244" s="5" t="s">
         <v>5</v>
@@ -4228,10 +4231,10 @@
     </row>
     <row r="245" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B245" s="7" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C245" s="5" t="s">
         <v>5</v>
@@ -4239,10 +4242,10 @@
     </row>
     <row r="246" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B246" s="7" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C246" s="5" t="s">
         <v>5</v>
@@ -4250,10 +4253,10 @@
     </row>
     <row r="247" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B247" s="7" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C247" s="5" t="s">
         <v>5</v>
@@ -4261,10 +4264,10 @@
     </row>
     <row r="248" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B248" s="7" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C248" s="5" t="s">
         <v>5</v>
@@ -4272,10 +4275,10 @@
     </row>
     <row r="249" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B249" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C249" s="5" t="s">
         <v>5</v>
@@ -4283,10 +4286,10 @@
     </row>
     <row r="250" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B250" s="7" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C250" s="5" t="s">
         <v>5</v>
@@ -4294,10 +4297,10 @@
     </row>
     <row r="251" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B251" s="7" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C251" s="5" t="s">
         <v>5</v>
@@ -4305,10 +4308,10 @@
     </row>
     <row r="252" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B252" s="7" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C252" s="5" t="s">
         <v>5</v>
@@ -4316,10 +4319,10 @@
     </row>
     <row r="253" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B253" s="7" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C253" s="5" t="s">
         <v>5</v>
@@ -4327,10 +4330,10 @@
     </row>
     <row r="254" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B254" s="7" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C254" s="5" t="s">
         <v>5</v>
@@ -4338,10 +4341,10 @@
     </row>
     <row r="255" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B255" s="7" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C255" s="5" t="s">
         <v>5</v>
@@ -4349,10 +4352,10 @@
     </row>
     <row r="256" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B256" s="7" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C256" s="5" t="s">
         <v>5</v>
@@ -4360,10 +4363,10 @@
     </row>
     <row r="257" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B257" s="7" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C257" s="5" t="s">
         <v>5</v>
@@ -4371,10 +4374,10 @@
     </row>
     <row r="258" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B258" s="7" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C258" s="5" t="s">
         <v>5</v>
@@ -4382,10 +4385,10 @@
     </row>
     <row r="259" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B259" s="7" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C259" s="5" t="s">
         <v>5</v>
@@ -4393,10 +4396,10 @@
     </row>
     <row r="260" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B260" s="7" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C260" s="5" t="s">
         <v>5</v>
@@ -4404,10 +4407,10 @@
     </row>
     <row r="261" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B261" s="7" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C261" s="5" t="s">
         <v>5</v>
@@ -4415,10 +4418,10 @@
     </row>
     <row r="262" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B262" s="7" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C262" s="5" t="s">
         <v>5</v>
@@ -4426,10 +4429,10 @@
     </row>
     <row r="263" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B263" s="7" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C263" s="5" t="s">
         <v>5</v>
@@ -4437,10 +4440,10 @@
     </row>
     <row r="264" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B264" s="7" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C264" s="5" t="s">
         <v>5</v>
@@ -4448,10 +4451,10 @@
     </row>
     <row r="265" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B265" s="7" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C265" s="5" t="s">
         <v>5</v>
@@ -4459,10 +4462,10 @@
     </row>
     <row r="266" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B266" s="7" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C266" s="5" t="s">
         <v>5</v>
@@ -4470,10 +4473,10 @@
     </row>
     <row r="267" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B267" s="7" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C267" s="5" t="s">
         <v>5</v>
@@ -4481,10 +4484,10 @@
     </row>
     <row r="268" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B268" s="7" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C268" s="5" t="s">
         <v>5</v>
@@ -4492,10 +4495,10 @@
     </row>
     <row r="269" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B269" s="7" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C269" s="5" t="s">
         <v>5</v>
@@ -4503,10 +4506,10 @@
     </row>
     <row r="270" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B270" s="7" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C270" s="5" t="s">
         <v>5</v>
@@ -4514,7 +4517,7 @@
     </row>
     <row r="271" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B271" s="7" t="s">
         <v>89</v>
@@ -4525,10 +4528,10 @@
     </row>
     <row r="272" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B272" s="7" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C272" s="5" t="s">
         <v>5</v>
@@ -4544,10 +4547,10 @@
     </row>
     <row r="275" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="6" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B275" s="7" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C275" s="5" t="s">
         <v>5</v>
@@ -4555,10 +4558,10 @@
     </row>
     <row r="276" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="6" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B276" s="7" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C276" s="5" t="s">
         <v>5</v>
@@ -4566,10 +4569,10 @@
     </row>
     <row r="277" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="6" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B277" s="7" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C277" s="5" t="s">
         <v>5</v>
@@ -4577,10 +4580,10 @@
     </row>
     <row r="278" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="6" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B278" s="7" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C278" s="5" t="s">
         <v>5</v>
@@ -4588,10 +4591,10 @@
     </row>
     <row r="279" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="6" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B279" s="7" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C279" s="5" t="s">
         <v>5</v>
@@ -4599,10 +4602,10 @@
     </row>
     <row r="280" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="6" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B280" s="7" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C280" s="5" t="s">
         <v>5</v>
@@ -4610,10 +4613,10 @@
     </row>
     <row r="281" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="6" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B281" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C281" s="5" t="s">
         <v>5</v>
@@ -4621,10 +4624,10 @@
     </row>
     <row r="282" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="6" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B282" s="7" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C282" s="5" t="s">
         <v>5</v>
@@ -4632,10 +4635,10 @@
     </row>
     <row r="283" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="6" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B283" s="7" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C283" s="5" t="s">
         <v>5</v>
@@ -4643,10 +4646,10 @@
     </row>
     <row r="284" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="6" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B284" s="7" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C284" s="5" t="s">
         <v>5</v>
@@ -4654,10 +4657,10 @@
     </row>
     <row r="285" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="6" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B285" s="7" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C285" s="5" t="s">
         <v>5</v>
@@ -4665,10 +4668,10 @@
     </row>
     <row r="286" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="6" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B286" s="7" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C286" s="5" t="s">
         <v>5</v>
@@ -4676,10 +4679,10 @@
     </row>
     <row r="287" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="6" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B287" s="7" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C287" s="5" t="s">
         <v>5</v>
@@ -4687,10 +4690,10 @@
     </row>
     <row r="288" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="6" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B288" s="7" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C288" s="5" t="s">
         <v>5</v>
@@ -4698,10 +4701,10 @@
     </row>
     <row r="289" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="6" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B289" s="7" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C289" s="5" t="s">
         <v>5</v>
@@ -4709,10 +4712,10 @@
     </row>
     <row r="290" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="6" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B290" s="7" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C290" s="5" t="s">
         <v>5</v>
@@ -4720,10 +4723,10 @@
     </row>
     <row r="291" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="6" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B291" s="7" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C291" s="5" t="s">
         <v>5</v>
@@ -4731,10 +4734,10 @@
     </row>
     <row r="292" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="6" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B292" s="7" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C292" s="5" t="s">
         <v>5</v>
@@ -4742,10 +4745,10 @@
     </row>
     <row r="293" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="6" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B293" s="7" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C293" s="5" t="s">
         <v>5</v>
@@ -4761,10 +4764,10 @@
     </row>
     <row r="296" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B296" s="7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C296" s="5" t="s">
         <v>8</v>
@@ -4772,10 +4775,10 @@
     </row>
     <row r="297" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B297" s="7" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C297" s="5" t="s">
         <v>8</v>
@@ -4783,10 +4786,10 @@
     </row>
     <row r="298" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B298" s="7" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C298" s="5" t="s">
         <v>8</v>
@@ -4794,10 +4797,10 @@
     </row>
     <row r="299" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B299" s="7" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C299" s="5" t="s">
         <v>5</v>
@@ -4805,10 +4808,10 @@
     </row>
     <row r="300" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B300" s="7" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C300" s="5" t="s">
         <v>5</v>
@@ -4816,10 +4819,10 @@
     </row>
     <row r="301" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B301" s="7" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C301" s="5" t="s">
         <v>5</v>
@@ -4827,10 +4830,10 @@
     </row>
     <row r="302" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B302" s="7" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C302" s="5" t="s">
         <v>5</v>
@@ -4838,10 +4841,10 @@
     </row>
     <row r="303" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B303" s="7" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C303" s="5" t="s">
         <v>5</v>
@@ -4849,10 +4852,10 @@
     </row>
     <row r="304" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B304" s="7" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C304" s="5" t="s">
         <v>5</v>
@@ -4860,10 +4863,10 @@
     </row>
     <row r="305" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B305" s="7" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C305" s="5" t="s">
         <v>5</v>
@@ -4871,10 +4874,10 @@
     </row>
     <row r="306" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B306" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C306" s="5" t="s">
         <v>5</v>
@@ -4882,10 +4885,10 @@
     </row>
     <row r="307" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B307" s="7" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C307" s="5" t="s">
         <v>5</v>
@@ -4893,10 +4896,10 @@
     </row>
     <row r="308" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B308" s="7" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C308" s="5" t="s">
         <v>5</v>
@@ -4904,10 +4907,10 @@
     </row>
     <row r="309" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B309" s="9" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C309" s="5" t="s">
         <v>5</v>
@@ -4915,10 +4918,10 @@
     </row>
     <row r="310" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B310" s="7" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C310" s="5" t="s">
         <v>5</v>
@@ -4926,10 +4929,10 @@
     </row>
     <row r="311" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B311" s="7" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C311" s="5" t="s">
         <v>5</v>
@@ -4937,10 +4940,10 @@
     </row>
     <row r="312" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B312" s="7" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C312" s="5" t="s">
         <v>5</v>
@@ -4948,10 +4951,10 @@
     </row>
     <row r="313" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B313" s="7" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C313" s="5" t="s">
         <v>5</v>
@@ -4959,10 +4962,10 @@
     </row>
     <row r="314" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B314" s="7" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C314" s="5" t="s">
         <v>5</v>
@@ -4970,10 +4973,10 @@
     </row>
     <row r="315" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B315" s="7" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C315" s="5" t="s">
         <v>5</v>
@@ -4981,10 +4984,10 @@
     </row>
     <row r="316" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B316" s="7" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C316" s="5" t="s">
         <v>5</v>
@@ -4992,10 +4995,10 @@
     </row>
     <row r="317" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B317" s="7" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C317" s="5" t="s">
         <v>5</v>
@@ -5003,10 +5006,10 @@
     </row>
     <row r="318" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B318" s="7" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C318" s="5" t="s">
         <v>5</v>
@@ -5014,10 +5017,10 @@
     </row>
     <row r="319" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B319" s="7" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C319" s="5" t="s">
         <v>5</v>
@@ -5025,10 +5028,10 @@
     </row>
     <row r="320" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B320" s="7" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C320" s="5" t="s">
         <v>5</v>
@@ -5036,10 +5039,10 @@
     </row>
     <row r="321" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B321" s="7" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C321" s="5" t="s">
         <v>5</v>
@@ -5047,10 +5050,10 @@
     </row>
     <row r="322" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B322" s="7" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C322" s="5" t="s">
         <v>5</v>
@@ -5058,10 +5061,10 @@
     </row>
     <row r="323" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B323" s="7" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C323" s="5" t="s">
         <v>5</v>
@@ -5069,10 +5072,10 @@
     </row>
     <row r="324" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B324" s="7" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C324" s="5" t="s">
         <v>5</v>
@@ -5080,10 +5083,10 @@
     </row>
     <row r="325" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B325" s="7" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C325" s="5" t="s">
         <v>5</v>
@@ -5091,10 +5094,10 @@
     </row>
     <row r="326" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B326" s="7" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C326" s="5" t="s">
         <v>5</v>
@@ -5102,10 +5105,10 @@
     </row>
     <row r="327" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B327" s="7" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C327" s="5" t="s">
         <v>5</v>
@@ -5113,10 +5116,10 @@
     </row>
     <row r="328" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B328" s="7" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C328" s="5" t="s">
         <v>5</v>
@@ -5124,10 +5127,10 @@
     </row>
     <row r="329" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B329" s="7" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C329" s="5" t="s">
         <v>5</v>
@@ -5135,10 +5138,10 @@
     </row>
     <row r="330" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B330" s="7" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C330" s="5" t="s">
         <v>5</v>
@@ -5146,10 +5149,10 @@
     </row>
     <row r="331" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B331" s="7" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C331" s="5" t="s">
         <v>5</v>
@@ -5157,10 +5160,10 @@
     </row>
     <row r="332" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B332" s="7" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C332" s="5" t="s">
         <v>5</v>
@@ -5168,10 +5171,10 @@
     </row>
     <row r="333" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="6" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B333" s="7" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C333" s="5" t="s">
         <v>5</v>
@@ -5187,10 +5190,10 @@
     </row>
     <row r="336" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B336" s="7" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C336" s="5" t="s">
         <v>5</v>
@@ -5198,10 +5201,10 @@
     </row>
     <row r="337" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B337" s="7" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C337" s="5" t="s">
         <v>5</v>
@@ -5209,10 +5212,10 @@
     </row>
     <row r="338" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B338" s="7" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C338" s="5" t="s">
         <v>5</v>
@@ -5220,10 +5223,10 @@
     </row>
     <row r="339" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B339" s="7" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C339" s="5" t="s">
         <v>5</v>
@@ -5231,10 +5234,10 @@
     </row>
     <row r="340" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B340" s="7" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C340" s="5" t="s">
         <v>5</v>
@@ -5242,10 +5245,10 @@
     </row>
     <row r="341" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B341" s="7" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C341" s="5" t="s">
         <v>5</v>
@@ -5253,10 +5256,10 @@
     </row>
     <row r="342" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B342" s="7" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C342" s="5" t="s">
         <v>5</v>
@@ -5264,10 +5267,10 @@
     </row>
     <row r="343" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B343" s="7" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C343" s="5" t="s">
         <v>5</v>
@@ -5275,10 +5278,10 @@
     </row>
     <row r="344" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B344" s="9" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C344" s="5" t="s">
         <v>5</v>
@@ -5286,10 +5289,10 @@
     </row>
     <row r="345" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B345" s="7" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C345" s="5" t="s">
         <v>5</v>
@@ -5297,10 +5300,10 @@
     </row>
     <row r="346" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B346" s="7" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C346" s="5" t="s">
         <v>5</v>
@@ -5308,10 +5311,10 @@
     </row>
     <row r="347" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B347" s="7" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C347" s="5" t="s">
         <v>5</v>
@@ -5319,10 +5322,10 @@
     </row>
     <row r="348" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B348" s="7" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C348" s="5" t="s">
         <v>5</v>
@@ -5330,10 +5333,10 @@
     </row>
     <row r="349" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B349" s="7" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C349" s="5" t="s">
         <v>5</v>
@@ -5341,10 +5344,10 @@
     </row>
     <row r="350" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B350" s="7" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C350" s="5" t="s">
         <v>5</v>
@@ -5352,10 +5355,10 @@
     </row>
     <row r="351" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B351" s="7" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C351" s="5" t="s">
         <v>5</v>
@@ -5363,10 +5366,10 @@
     </row>
     <row r="352" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B352" s="7" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C352" s="5" t="s">
         <v>5</v>
@@ -5374,10 +5377,10 @@
     </row>
     <row r="353" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B353" s="7" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C353" s="5" t="s">
         <v>5</v>
@@ -5393,10 +5396,10 @@
     </row>
     <row r="356" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B356" s="7" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C356" s="5" t="s">
         <v>5</v>
@@ -5404,10 +5407,10 @@
     </row>
     <row r="357" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B357" s="7" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C357" s="5" t="s">
         <v>5</v>
@@ -5415,10 +5418,10 @@
     </row>
     <row r="358" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B358" s="7" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C358" s="5" t="s">
         <v>5</v>
@@ -5426,10 +5429,10 @@
     </row>
     <row r="359" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B359" s="7" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C359" s="5" t="s">
         <v>5</v>
@@ -5437,10 +5440,10 @@
     </row>
     <row r="360" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B360" s="7" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C360" s="5" t="s">
         <v>5</v>
@@ -5448,10 +5451,10 @@
     </row>
     <row r="361" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B361" s="7" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C361" s="5" t="s">
         <v>5</v>
@@ -5459,10 +5462,10 @@
     </row>
     <row r="362" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B362" s="7" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C362" s="5" t="s">
         <v>5</v>
@@ -5470,10 +5473,10 @@
     </row>
     <row r="363" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B363" s="7" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C363" s="5" t="s">
         <v>5</v>
@@ -5481,10 +5484,10 @@
     </row>
     <row r="364" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B364" s="7" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C364" s="5" t="s">
         <v>5</v>
@@ -5492,10 +5495,10 @@
     </row>
     <row r="365" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B365" s="7" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C365" s="5" t="s">
         <v>5</v>
@@ -5503,10 +5506,10 @@
     </row>
     <row r="366" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B366" s="7" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C366" s="5" t="s">
         <v>5</v>
@@ -5514,10 +5517,10 @@
     </row>
     <row r="367" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B367" s="7" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C367" s="5" t="s">
         <v>5</v>
@@ -5525,10 +5528,10 @@
     </row>
     <row r="368" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B368" s="7" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C368" s="5" t="s">
         <v>5</v>
@@ -5536,10 +5539,10 @@
     </row>
     <row r="369" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B369" s="7" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C369" s="5" t="s">
         <v>5</v>
@@ -5547,10 +5550,10 @@
     </row>
     <row r="370" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B370" s="7" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C370" s="5" t="s">
         <v>5</v>
@@ -5558,10 +5561,10 @@
     </row>
     <row r="371" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B371" s="7" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C371" s="5" t="s">
         <v>5</v>
@@ -5569,10 +5572,10 @@
     </row>
     <row r="372" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B372" s="7" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C372" s="5" t="s">
         <v>5</v>
@@ -5580,10 +5583,10 @@
     </row>
     <row r="373" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B373" s="7" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C373" s="5" t="s">
         <v>5</v>
@@ -5591,10 +5594,10 @@
     </row>
     <row r="374" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B374" s="7" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C374" s="5" t="s">
         <v>5</v>
@@ -5602,10 +5605,10 @@
     </row>
     <row r="375" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B375" s="7" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C375" s="5" t="s">
         <v>5</v>
@@ -5613,10 +5616,10 @@
     </row>
     <row r="376" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B376" s="7" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C376" s="5" t="s">
         <v>5</v>
@@ -5624,10 +5627,10 @@
     </row>
     <row r="377" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B377" s="7" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C377" s="5" t="s">
         <v>5</v>
@@ -5635,10 +5638,10 @@
     </row>
     <row r="378" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B378" s="7" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C378" s="5" t="s">
         <v>5</v>
@@ -5646,10 +5649,10 @@
     </row>
     <row r="379" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B379" s="7" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C379" s="5" t="s">
         <v>5</v>
@@ -5657,10 +5660,10 @@
     </row>
     <row r="380" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B380" s="7" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C380" s="5" t="s">
         <v>5</v>
@@ -5668,10 +5671,10 @@
     </row>
     <row r="381" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B381" s="7" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C381" s="5" t="s">
         <v>5</v>
@@ -5679,10 +5682,10 @@
     </row>
     <row r="382" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B382" s="7" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C382" s="5" t="s">
         <v>5</v>
@@ -5690,10 +5693,10 @@
     </row>
     <row r="383" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B383" s="7" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C383" s="5" t="s">
         <v>5</v>
@@ -5701,10 +5704,10 @@
     </row>
     <row r="384" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B384" s="7" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C384" s="5" t="s">
         <v>5</v>
@@ -5712,10 +5715,10 @@
     </row>
     <row r="385" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B385" s="7" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C385" s="5" t="s">
         <v>5</v>
@@ -5723,10 +5726,10 @@
     </row>
     <row r="386" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B386" s="7" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C386" s="5" t="s">
         <v>5</v>
@@ -5734,10 +5737,10 @@
     </row>
     <row r="387" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B387" s="7" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C387" s="5" t="s">
         <v>5</v>
@@ -5745,10 +5748,10 @@
     </row>
     <row r="388" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B388" s="7" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C388" s="5" t="s">
         <v>5</v>
@@ -5756,10 +5759,10 @@
     </row>
     <row r="389" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B389" s="7" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C389" s="5" t="s">
         <v>5</v>
@@ -5767,10 +5770,10 @@
     </row>
     <row r="390" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B390" s="7" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C390" s="5" t="s">
         <v>5</v>
@@ -5778,10 +5781,10 @@
     </row>
     <row r="391" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B391" s="7" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C391" s="5" t="s">
         <v>5</v>
@@ -5789,10 +5792,10 @@
     </row>
     <row r="392" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B392" s="7" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C392" s="5" t="s">
         <v>5</v>
@@ -5800,10 +5803,10 @@
     </row>
     <row r="393" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B393" s="7" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C393" s="5" t="s">
         <v>5</v>
@@ -5811,10 +5814,10 @@
     </row>
     <row r="394" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B394" s="7" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C394" s="5" t="s">
         <v>5</v>
@@ -5822,10 +5825,10 @@
     </row>
     <row r="395" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B395" s="7" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C395" s="5" t="s">
         <v>5</v>
@@ -5833,10 +5836,10 @@
     </row>
     <row r="396" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B396" s="7" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C396" s="5" t="s">
         <v>5</v>
@@ -5844,10 +5847,10 @@
     </row>
     <row r="397" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B397" s="7" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C397" s="5" t="s">
         <v>5</v>
@@ -5855,10 +5858,10 @@
     </row>
     <row r="398" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B398" s="7" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C398" s="5" t="s">
         <v>5</v>
@@ -5866,10 +5869,10 @@
     </row>
     <row r="399" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B399" s="7" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C399" s="5" t="s">
         <v>5</v>
@@ -5885,10 +5888,10 @@
     </row>
     <row r="402" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="6" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B402" s="7" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C402" s="5" t="s">
         <v>5</v>
@@ -5896,10 +5899,10 @@
     </row>
     <row r="403" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="6" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B403" s="7" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C403" s="5" t="s">
         <v>5</v>
@@ -5907,10 +5910,10 @@
     </row>
     <row r="404" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="6" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B404" s="7" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C404" s="5" t="s">
         <v>5</v>
@@ -5918,7 +5921,7 @@
     </row>
     <row r="405" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="6" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B405" s="7" t="s">
         <v>91</v>
@@ -5929,10 +5932,10 @@
     </row>
     <row r="406" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="6" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B406" s="7" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C406" s="5" t="s">
         <v>5</v>
@@ -5940,10 +5943,10 @@
     </row>
     <row r="407" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="6" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B407" s="7" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C407" s="5" t="s">
         <v>5</v>
@@ -5959,10 +5962,10 @@
     </row>
     <row r="410" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B410" s="7" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C410" s="5" t="s">
         <v>5</v>
@@ -5970,10 +5973,10 @@
     </row>
     <row r="411" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B411" s="7" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C411" s="5" t="s">
         <v>5</v>
@@ -5981,10 +5984,10 @@
     </row>
     <row r="412" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B412" s="7" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C412" s="5" t="s">
         <v>5</v>
@@ -5992,10 +5995,10 @@
     </row>
     <row r="413" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B413" s="7" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C413" s="5" t="s">
         <v>5</v>
@@ -6003,10 +6006,10 @@
     </row>
     <row r="414" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B414" s="7" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C414" s="5" t="s">
         <v>5</v>
@@ -6014,10 +6017,10 @@
     </row>
     <row r="415" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B415" s="7" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C415" s="5" t="s">
         <v>5</v>
@@ -6025,10 +6028,10 @@
     </row>
     <row r="416" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B416" s="7" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C416" s="5" t="s">
         <v>5</v>
@@ -6036,10 +6039,10 @@
     </row>
     <row r="417" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B417" s="7" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C417" s="5" t="s">
         <v>5</v>
@@ -6047,10 +6050,10 @@
     </row>
     <row r="418" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B418" s="7" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C418" s="5" t="s">
         <v>5</v>
@@ -6058,10 +6061,10 @@
     </row>
     <row r="419" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B419" s="7" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C419" s="5" t="s">
         <v>5</v>
@@ -6069,10 +6072,10 @@
     </row>
     <row r="420" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B420" s="7" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C420" s="5" t="s">
         <v>5</v>
@@ -6080,10 +6083,10 @@
     </row>
     <row r="421" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B421" s="7" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C421" s="5" t="s">
         <v>5</v>
@@ -6091,10 +6094,10 @@
     </row>
     <row r="422" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B422" s="7" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C422" s="5" t="s">
         <v>5</v>
@@ -6102,10 +6105,10 @@
     </row>
     <row r="423" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B423" s="7" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C423" s="5" t="s">
         <v>5</v>
@@ -6113,10 +6116,10 @@
     </row>
     <row r="424" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B424" s="7" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C424" s="5" t="s">
         <v>5</v>
@@ -6124,10 +6127,10 @@
     </row>
     <row r="425" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B425" s="7" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C425" s="5" t="s">
         <v>5</v>
@@ -6135,10 +6138,10 @@
     </row>
     <row r="426" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B426" s="7" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C426" s="5" t="s">
         <v>5</v>
@@ -6146,10 +6149,10 @@
     </row>
     <row r="427" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B427" s="7" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C427" s="5" t="s">
         <v>5</v>
@@ -6157,10 +6160,10 @@
     </row>
     <row r="428" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B428" s="7" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C428" s="5" t="s">
         <v>5</v>
@@ -6168,10 +6171,10 @@
     </row>
     <row r="429" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B429" s="7" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C429" s="5" t="s">
         <v>5</v>
@@ -6179,10 +6182,10 @@
     </row>
     <row r="430" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B430" s="7" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C430" s="5" t="s">
         <v>5</v>
@@ -6190,10 +6193,10 @@
     </row>
     <row r="431" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B431" s="7" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C431" s="5" t="s">
         <v>5</v>
@@ -6201,10 +6204,10 @@
     </row>
     <row r="432" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B432" s="7" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C432" s="5" t="s">
         <v>5</v>
@@ -6212,10 +6215,10 @@
     </row>
     <row r="433" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B433" s="7" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C433" s="5" t="s">
         <v>5</v>
@@ -6223,10 +6226,10 @@
     </row>
     <row r="434" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B434" s="7" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C434" s="5" t="s">
         <v>5</v>
@@ -6234,10 +6237,10 @@
     </row>
     <row r="435" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B435" s="7" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C435" s="5" t="s">
         <v>5</v>
@@ -6245,10 +6248,10 @@
     </row>
     <row r="436" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B436" s="7" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C436" s="5" t="s">
         <v>5</v>
@@ -6256,10 +6259,10 @@
     </row>
     <row r="437" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B437" s="7" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="C437" s="5" t="s">
         <v>5</v>
@@ -6267,10 +6270,10 @@
     </row>
     <row r="438" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B438" s="7" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C438" s="5" t="s">
         <v>5</v>
@@ -6278,10 +6281,10 @@
     </row>
     <row r="439" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B439" s="7" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C439" s="5" t="s">
         <v>5</v>
@@ -6289,10 +6292,10 @@
     </row>
     <row r="440" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B440" s="7" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C440" s="5" t="s">
         <v>5</v>
@@ -6300,10 +6303,10 @@
     </row>
     <row r="441" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B441" s="7" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C441" s="5" t="s">
         <v>5</v>
@@ -6311,10 +6314,10 @@
     </row>
     <row r="442" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B442" s="7" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C442" s="5" t="s">
         <v>5</v>
@@ -6322,10 +6325,10 @@
     </row>
     <row r="443" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B443" s="7" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C443" s="5" t="s">
         <v>5</v>
@@ -6333,10 +6336,10 @@
     </row>
     <row r="444" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B444" s="7" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C444" s="5" t="s">
         <v>5</v>
@@ -6344,10 +6347,10 @@
     </row>
     <row r="445" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B445" s="7" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C445" s="5" t="s">
         <v>5</v>
@@ -6355,10 +6358,10 @@
     </row>
     <row r="446" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B446" s="7" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C446" s="5" t="s">
         <v>5</v>
@@ -6366,10 +6369,10 @@
     </row>
     <row r="447" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B447" s="7" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C447" s="5" t="s">
         <v>5</v>
@@ -6377,10 +6380,10 @@
     </row>
     <row r="448" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B448" s="7" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C448" s="5" t="s">
         <v>5</v>
@@ -6388,10 +6391,10 @@
     </row>
     <row r="449" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B449" s="7" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C449" s="5" t="s">
         <v>5</v>
@@ -6399,10 +6402,10 @@
     </row>
     <row r="450" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B450" s="7" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C450" s="5" t="s">
         <v>5</v>
@@ -6410,10 +6413,10 @@
     </row>
     <row r="451" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B451" s="7" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C451" s="5" t="s">
         <v>5</v>
@@ -6421,10 +6424,10 @@
     </row>
     <row r="452" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B452" s="7" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C452" s="5" t="s">
         <v>5</v>
@@ -6432,10 +6435,10 @@
     </row>
     <row r="453" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B453" s="7" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C453" s="5" t="s">
         <v>5</v>
@@ -6443,10 +6446,10 @@
     </row>
     <row r="454" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B454" s="7" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C454" s="5" t="s">
         <v>5</v>
@@ -6454,10 +6457,10 @@
     </row>
     <row r="455" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B455" s="7" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C455" s="5" t="s">
         <v>5</v>
@@ -6465,10 +6468,10 @@
     </row>
     <row r="456" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B456" s="7" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C456" s="5" t="s">
         <v>5</v>
@@ -6476,10 +6479,10 @@
     </row>
     <row r="457" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B457" s="7" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C457" s="5" t="s">
         <v>5</v>
@@ -6487,10 +6490,10 @@
     </row>
     <row r="458" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B458" s="7" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C458" s="5" t="s">
         <v>5</v>
@@ -6498,10 +6501,10 @@
     </row>
     <row r="459" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B459" s="7" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C459" s="5" t="s">
         <v>5</v>
@@ -6509,10 +6512,10 @@
     </row>
     <row r="460" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B460" s="7" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C460" s="5" t="s">
         <v>5</v>
@@ -6520,10 +6523,10 @@
     </row>
     <row r="461" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B461" s="7" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C461" s="5" t="s">
         <v>5</v>
@@ -6531,10 +6534,10 @@
     </row>
     <row r="462" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B462" s="7" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C462" s="5" t="s">
         <v>5</v>
@@ -6542,10 +6545,10 @@
     </row>
     <row r="463" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B463" s="7" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C463" s="5" t="s">
         <v>5</v>
@@ -6553,10 +6556,10 @@
     </row>
     <row r="464" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B464" s="7" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C464" s="5" t="s">
         <v>5</v>
@@ -6564,10 +6567,10 @@
     </row>
     <row r="465" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B465" s="7" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C465" s="5" t="s">
         <v>5</v>
@@ -6575,10 +6578,10 @@
     </row>
     <row r="466" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B466" s="7" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C466" s="5" t="s">
         <v>5</v>
@@ -6586,10 +6589,10 @@
     </row>
     <row r="467" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B467" s="7" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C467" s="5" t="s">
         <v>5</v>
@@ -6597,10 +6600,10 @@
     </row>
     <row r="468" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B468" s="7" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C468" s="5" t="s">
         <v>5</v>
@@ -6608,10 +6611,10 @@
     </row>
     <row r="469" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B469" s="7" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="C469" s="5" t="s">
         <v>5</v>
@@ -6628,10 +6631,10 @@
     </row>
     <row r="472" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="6" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B472" s="7" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C472" s="5" t="s">
         <v>5</v>
@@ -6639,10 +6642,10 @@
     </row>
     <row r="473" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="6" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B473" s="7" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C473" s="5" t="s">
         <v>5</v>
@@ -6650,10 +6653,10 @@
     </row>
     <row r="474" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A474" s="6" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B474" s="7" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C474" s="5" t="s">
         <v>5</v>
@@ -6661,10 +6664,10 @@
     </row>
     <row r="475" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="6" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B475" s="7" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C475" s="5" t="s">
         <v>5</v>
@@ -6672,10 +6675,10 @@
     </row>
     <row r="476" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A476" s="6" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B476" s="7" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C476" s="5" t="s">
         <v>5</v>
@@ -6683,10 +6686,10 @@
     </row>
     <row r="477" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="6" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B477" s="7" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C477" s="5" t="s">
         <v>5</v>
@@ -6694,10 +6697,10 @@
     </row>
     <row r="478" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A478" s="6" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B478" s="7" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C478" s="5" t="s">
         <v>5</v>
@@ -6705,10 +6708,10 @@
     </row>
     <row r="479" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="6" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B479" s="7" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C479" s="5" t="s">
         <v>5</v>
@@ -6716,10 +6719,10 @@
     </row>
     <row r="480" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="6" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B480" s="7" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C480" s="5" t="s">
         <v>5</v>
@@ -6727,10 +6730,10 @@
     </row>
     <row r="481" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="6" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B481" s="7" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C481" s="5" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
array sort zero one two
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1668,11 +1668,11 @@
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A169" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D177" activeCellId="0" sqref="D177"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="123"/>
@@ -1746,7 +1746,7 @@
         <v>11</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
first and last position
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1668,11 +1668,11 @@
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D60" activeCellId="0" sqref="D60"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C101" activeCellId="0" sqref="C101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="123"/>
@@ -2715,7 +2715,7 @@
         <v>100</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
value equal to index
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1669,10 +1669,10 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C101" activeCellId="0" sqref="C101"/>
+      <selection pane="topLeft" activeCell="C102" activeCellId="0" sqref="C102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.62109375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="123"/>
@@ -2726,7 +2726,7 @@
         <v>101</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
find middle in stack
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1668,11 +1668,11 @@
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C102" activeCellId="0" sqref="C102"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A277" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D299" activeCellId="0" sqref="D299"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.62109375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.62890625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="123"/>
@@ -4803,7 +4803,7 @@
         <v>292</v>
       </c>
       <c r="C299" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
reverse order level traversing
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1668,11 +1668,11 @@
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A124" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D142" activeCellId="0" sqref="D142"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A175" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D178" activeCellId="0" sqref="D178"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.63671875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.640625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="123"/>
@@ -3526,7 +3526,7 @@
         <v>176</v>
       </c>
       <c r="C178" s="5" t="s">
-        <v>5</v>
+        <v>175</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
hight of the tree
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1668,11 +1668,11 @@
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A175" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D178" activeCellId="0" sqref="D178"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A175" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D179" activeCellId="0" sqref="D179"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.640625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="123"/>
@@ -3537,7 +3537,7 @@
         <v>177</v>
       </c>
       <c r="C179" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
detect first element in a loop
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1668,11 +1668,11 @@
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A175" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D179" activeCellId="0" sqref="D179"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A112" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C143" activeCellId="0" sqref="C143"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.65625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="123"/>
@@ -3159,7 +3159,7 @@
         <v>141</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>